<commit_message>
Modified feature file data
</commit_message>
<xml_diff>
--- a/onboarding.specflow-master/MarsQA-1/SpecflowTests/Data/ProfileData.xlsx
+++ b/onboarding.specflow-master/MarsQA-1/SpecflowTests/Data/ProfileData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AdvancedTaskLevel1\onboarding.specflow-master\MarsQA-1\SpecflowTests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6663D844-9A31-4110-9C2C-CF1D4F9E119C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8648409C-8624-43AF-8E85-A72351B2EA5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{B4A64FCC-6ABA-4EDA-AE0D-C055547341E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>CollegeName</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>BE</t>
+  </si>
+  <si>
+    <t>UpdateCollege</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>M.B.A</t>
   </si>
 </sst>
 </file>
@@ -438,10 +447,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906F3707-5AE3-496A-8B92-4C599A851D5C}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,8 +496,26 @@
         <v>2015</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>2016</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>